<commit_message>
Pennink Series 2 done.
</commit_message>
<xml_diff>
--- a/Projects/Pennink-Model/cases/Series2/Series2.xlsx
+++ b/Projects/Pennink-Model/cases/Series2/Series2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Pennink-Model/cases/Series2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63202893-91EE-0C48-9EB3-EDDBC16746F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E637749-B1C9-E945-A6F9-39F9DE3A06C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11860" yWindow="-25980" windowWidth="30600" windowHeight="19860" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7360" yWindow="1700" windowWidth="28180" windowHeight="16980" tabRatio="751" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="GWF6" sheetId="9" r:id="rId3"/>
     <sheet name="GWT6" sheetId="10" r:id="rId4"/>
     <sheet name="PER" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId6"/>
+    <sheet name="PER (2)" sheetId="13" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_rch2">#REF!</definedName>
@@ -126,8 +127,81 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{165D8FC6-FBD1-5148-A2CC-E60CCB8DEA89}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Stress period nr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{DFA59D8D-F890-4A4F-8E81-FE46F2EF4A9D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Length of stress period
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(use consistent units)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{4CB9FF73-8F23-ED4D-8B40-D4C1494038FB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of time steps
+in each stress period</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{C611C11C-6118-4141-8D6E-686024196166}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Time step length multiplier to increase subsequent time step lengths during this stress period. It is used only if NSTP&gt;1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2491" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="415">
   <si>
     <t>ON / OFF</t>
   </si>
@@ -1360,6 +1434,18 @@
   </si>
   <si>
     <t>Photo</t>
+  </si>
+  <si>
+    <t>Pennink</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>NEWTON UNDER_RELAXATION</t>
+  </si>
+  <si>
+    <t>NO_PTC</t>
   </si>
 </sst>
 </file>
@@ -1861,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2312,11 +2398,11 @@
         <v>305</v>
       </c>
       <c r="B30" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>306</v>
@@ -3422,8 +3508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView topLeftCell="A6" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3594,8 +3680,8 @@
       <c r="B15" t="s">
         <v>112</v>
       </c>
-      <c r="C15" t="s">
-        <v>19</v>
+      <c r="C15" s="9" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -5706,8 +5792,8 @@
       <c r="B218" t="s">
         <v>43</v>
       </c>
-      <c r="C218" t="s">
-        <v>19</v>
+      <c r="C218" s="9" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.15">
@@ -6608,8 +6694,8 @@
       <c r="B306" t="s">
         <v>43</v>
       </c>
-      <c r="C306" t="s">
-        <v>19</v>
+      <c r="C306" s="9" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.15">
@@ -8405,8 +8491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06ADD67-459A-3448-A388-0C190A7D0288}">
   <dimension ref="A1:D315"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A10" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8617,8 +8703,8 @@
       <c r="B19" t="s">
         <v>112</v>
       </c>
-      <c r="C19" t="s">
-        <v>19</v>
+      <c r="C19" s="9" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -11714,9 +11800,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -11727,7 +11813,7 @@
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
@@ -11736,7 +11822,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -11758,8 +11844,14 @@
       <c r="G2" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H2" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>0</v>
       </c>
@@ -11767,10 +11859,11 @@
         <v>390</v>
       </c>
       <c r="C3">
-        <v>40.00000000007276</v>
+        <v>10</v>
       </c>
       <c r="D3" s="8">
-        <v>40.00000000007276</v>
+        <f>C3</f>
+        <v>10</v>
       </c>
       <c r="E3" s="8">
         <v>1</v>
@@ -11781,8 +11874,14 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -11790,10 +11889,11 @@
         <v>391</v>
       </c>
       <c r="C4">
-        <v>14.999999999781721</v>
+        <v>120</v>
       </c>
       <c r="D4" s="8">
-        <v>14.999999999781721</v>
+        <f t="shared" ref="D4:D5" si="0">C4</f>
+        <v>120</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
@@ -11804,166 +11904,43 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H4">
+        <f>SUM($C$3:C3)</f>
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="C5">
-        <v>25.000000000291038</v>
+        <v>120</v>
       </c>
       <c r="D5" s="8">
-        <v>25.000000000291038</v>
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>393</v>
-      </c>
-      <c r="C6">
-        <v>34.999999999818101</v>
-      </c>
-      <c r="D6" s="8">
-        <v>34.999999999818101</v>
-      </c>
-      <c r="E6" s="8">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>403</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>394</v>
-      </c>
-      <c r="C7">
-        <v>29.999999999890861</v>
-      </c>
-      <c r="D7" s="8">
-        <v>29.999999999890861</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>404</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>395</v>
-      </c>
-      <c r="C8">
-        <v>115.00000000029104</v>
-      </c>
-      <c r="D8" s="8">
-        <v>115.00000000029104</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>405</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>396</v>
-      </c>
-      <c r="C9">
-        <v>54.999999999854481</v>
-      </c>
-      <c r="D9" s="8">
-        <v>54.999999999854481</v>
-      </c>
-      <c r="E9" s="8">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>406</v>
-      </c>
-      <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>397</v>
-      </c>
-      <c r="C10">
-        <v>935.00000000014552</v>
-      </c>
-      <c r="D10" s="8">
-        <v>935.00000000014552</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>407</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11" s="8">
-        <v>10</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>408</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
+      <c r="H5">
+        <f>SUM($C$3:C4)</f>
+        <v>130</v>
+      </c>
+      <c r="I5">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -11975,6 +11952,336 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2467E7-2FD5-A243-B6F4-695802E8E562}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C3">
+        <v>40.00000000007276</v>
+      </c>
+      <c r="D3" s="8">
+        <v>40.00000000007276</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>400</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C4">
+        <v>14.999999999781721</v>
+      </c>
+      <c r="D4" s="8">
+        <v>14.999999999781721</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>401</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f>SUM($C$3:C3)</f>
+        <v>40.00000000007276</v>
+      </c>
+      <c r="I4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C5">
+        <v>25.000000000291038</v>
+      </c>
+      <c r="D5" s="8">
+        <v>25.000000000291038</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>402</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f>SUM($C$3:C4)</f>
+        <v>54.999999999854481</v>
+      </c>
+      <c r="I5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C6">
+        <v>34.999999999818101</v>
+      </c>
+      <c r="D6" s="8">
+        <v>34.999999999818101</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>403</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f>SUM($C$3:C5)</f>
+        <v>80.000000000145519</v>
+      </c>
+      <c r="I6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C7">
+        <v>29.999999999890861</v>
+      </c>
+      <c r="D7" s="8">
+        <v>29.999999999890861</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>404</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f>SUM($C$3:C6)</f>
+        <v>114.99999999996362</v>
+      </c>
+      <c r="I7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>395</v>
+      </c>
+      <c r="C8">
+        <v>115.00000000029104</v>
+      </c>
+      <c r="D8" s="8">
+        <v>115.00000000029104</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>405</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f>SUM($C$3:C7)</f>
+        <v>144.99999999985448</v>
+      </c>
+      <c r="I8">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>396</v>
+      </c>
+      <c r="C9">
+        <v>54.999999999854481</v>
+      </c>
+      <c r="D9" s="8">
+        <v>54.999999999854481</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>406</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f>SUM($C$3:C8)</f>
+        <v>260.00000000014552</v>
+      </c>
+      <c r="I9">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>397</v>
+      </c>
+      <c r="C10">
+        <v>935.00000000014552</v>
+      </c>
+      <c r="D10" s="8">
+        <v>935.00000000014552</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>407</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>SUM($C$3:C9)</f>
+        <v>315</v>
+      </c>
+      <c r="I10">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>408</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>SUM($C$3:C10)</f>
+        <v>1250.0000000001455</v>
+      </c>
+      <c r="I11">
+        <v>1250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4289E7A-CAF4-AC46-949F-DB1752B1DF3A}">
   <dimension ref="A1:D7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Pennink Series3 works, but convergence fails after about 30 time steps. That is with cell size 1 cm, with 0.5 cm it converges al the way through.
</commit_message>
<xml_diff>
--- a/Projects/Pennink-Model/cases/Series2/Series2.xlsx
+++ b/Projects/Pennink-Model/cases/Series2/Series2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Pennink-Model/cases/Series2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E637749-B1C9-E945-A6F9-39F9DE3A06C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA2083F-BF10-C84B-A004-579BF6B95D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="1700" windowWidth="28180" windowHeight="16980" tabRatio="751" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9820" yWindow="-24220" windowWidth="28180" windowHeight="16980" tabRatio="751" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="GWT6" sheetId="10" r:id="rId4"/>
     <sheet name="PER" sheetId="5" r:id="rId5"/>
     <sheet name="PER (2)" sheetId="13" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_rch2">#REF!</definedName>
@@ -201,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="447">
   <si>
     <t>ON / OFF</t>
   </si>
@@ -1355,24 +1354,6 @@
     <t>Minutes</t>
   </si>
   <si>
-    <t>m2/d</t>
-  </si>
-  <si>
-    <t>m2/s</t>
-  </si>
-  <si>
-    <t>m2/min</t>
-  </si>
-  <si>
-    <t>cm2/min</t>
-  </si>
-  <si>
-    <t>Henry problem by Modflow Development Team (2023) in Henry problem.</t>
-  </si>
-  <si>
-    <t>Used by GEO-SLOPE InternationalLit, Calgary, Alberta Canada in their paper.</t>
-  </si>
-  <si>
     <t>1904-09-01T09:00</t>
   </si>
   <si>
@@ -1446,6 +1427,120 @@
   </si>
   <si>
     <t>NO_PTC</t>
+  </si>
+  <si>
+    <t>ims</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>chd</t>
+  </si>
+  <si>
+    <t>dis</t>
+  </si>
+  <si>
+    <t>disu</t>
+  </si>
+  <si>
+    <t>disv</t>
+  </si>
+  <si>
+    <t>drn</t>
+  </si>
+  <si>
+    <t>evt</t>
+  </si>
+  <si>
+    <t>evta</t>
+  </si>
+  <si>
+    <t>ghb</t>
+  </si>
+  <si>
+    <t>gnc</t>
+  </si>
+  <si>
+    <t>hfb</t>
+  </si>
+  <si>
+    <t>ic</t>
+  </si>
+  <si>
+    <t>lak</t>
+  </si>
+  <si>
+    <t>maw</t>
+  </si>
+  <si>
+    <t>mvr</t>
+  </si>
+  <si>
+    <t>nam</t>
+  </si>
+  <si>
+    <t>npf</t>
+  </si>
+  <si>
+    <t>rch</t>
+  </si>
+  <si>
+    <t>rcha</t>
+  </si>
+  <si>
+    <t>riv</t>
+  </si>
+  <si>
+    <t>sfr</t>
+  </si>
+  <si>
+    <t>sto</t>
+  </si>
+  <si>
+    <t>uzf</t>
+  </si>
+  <si>
+    <t>wel</t>
+  </si>
+  <si>
+    <t>cnc</t>
+  </si>
+  <si>
+    <t>dsp</t>
+  </si>
+  <si>
+    <t>fmi</t>
+  </si>
+  <si>
+    <t>ist</t>
+  </si>
+  <si>
+    <t>lkt</t>
+  </si>
+  <si>
+    <t>mst</t>
+  </si>
+  <si>
+    <t>mvt</t>
+  </si>
+  <si>
+    <t>mwt</t>
+  </si>
+  <si>
+    <t>oc</t>
+  </si>
+  <si>
+    <t>sft</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>ssm</t>
+  </si>
+  <si>
+    <t>uzt</t>
   </si>
 </sst>
 </file>
@@ -1947,8 +2042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2674,8 +2769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9985BC8C-AF94-474C-A200-72B17F25D172}">
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:C80"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3136,6 +3231,38 @@
         <v>19</v>
       </c>
     </row>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>352</v>
@@ -3508,8 +3635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A326" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C344" sqref="C344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3681,7 +3808,7 @@
         <v>112</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -3966,8 +4093,8 @@
       <c r="B41" t="s">
         <v>30</v>
       </c>
-      <c r="C41" t="s">
-        <v>19</v>
+      <c r="C41" s="9" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -4076,8 +4203,8 @@
       <c r="B52" t="s">
         <v>31</v>
       </c>
-      <c r="C52" t="s">
-        <v>19</v>
+      <c r="C52" s="9" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -4230,8 +4357,8 @@
       <c r="B67" t="s">
         <v>31</v>
       </c>
-      <c r="C67" t="s">
-        <v>19</v>
+      <c r="C67" s="9" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -4417,8 +4544,8 @@
       <c r="B85" t="s">
         <v>31</v>
       </c>
-      <c r="C85" t="s">
-        <v>19</v>
+      <c r="C85" s="9" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -4604,8 +4731,8 @@
       <c r="B103" t="s">
         <v>31</v>
       </c>
-      <c r="C103" t="s">
-        <v>19</v>
+      <c r="C103" s="9" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
@@ -4780,8 +4907,8 @@
       <c r="B120" t="s">
         <v>31</v>
       </c>
-      <c r="C120" t="s">
-        <v>19</v>
+      <c r="C120" s="9" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
@@ -4956,8 +5083,8 @@
       <c r="B137" t="s">
         <v>31</v>
       </c>
-      <c r="C137" t="s">
-        <v>19</v>
+      <c r="C137" s="9" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
@@ -5143,8 +5270,8 @@
       <c r="B155" t="s">
         <v>31</v>
       </c>
-      <c r="C155" t="s">
-        <v>19</v>
+      <c r="C155" s="9" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.15">
@@ -5341,8 +5468,8 @@
       <c r="B174" t="s">
         <v>31</v>
       </c>
-      <c r="C174" t="s">
-        <v>19</v>
+      <c r="C174" s="9" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
@@ -5506,8 +5633,8 @@
       <c r="B190" t="s">
         <v>31</v>
       </c>
-      <c r="C190" t="s">
-        <v>19</v>
+      <c r="C190" s="9" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
@@ -5671,8 +5798,8 @@
       <c r="B206" t="s">
         <v>31</v>
       </c>
-      <c r="C206" t="s">
-        <v>19</v>
+      <c r="C206" s="9" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.15">
@@ -5793,7 +5920,7 @@
         <v>43</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.15">
@@ -5869,8 +5996,8 @@
       <c r="B226" t="s">
         <v>31</v>
       </c>
-      <c r="C226" t="s">
-        <v>19</v>
+      <c r="C226" s="9" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.15">
@@ -5924,8 +6051,8 @@
       <c r="B232" t="s">
         <v>31</v>
       </c>
-      <c r="C232" t="s">
-        <v>19</v>
+      <c r="C232" s="9" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.15">
@@ -6221,8 +6348,8 @@
       <c r="B260" t="s">
         <v>31</v>
       </c>
-      <c r="C260" t="s">
-        <v>19</v>
+      <c r="C260" s="9" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.15">
@@ -6485,8 +6612,8 @@
       <c r="B285" t="s">
         <v>31</v>
       </c>
-      <c r="C285" t="s">
-        <v>19</v>
+      <c r="C285" s="9" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.15">
@@ -6617,8 +6744,8 @@
       <c r="B298" t="s">
         <v>31</v>
       </c>
-      <c r="C298" t="s">
-        <v>19</v>
+      <c r="C298" s="9" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.15">
@@ -6695,7 +6822,7 @@
         <v>43</v>
       </c>
       <c r="C306" s="9" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.15">
@@ -6727,8 +6854,8 @@
       <c r="B309" t="s">
         <v>31</v>
       </c>
-      <c r="C309" t="s">
-        <v>19</v>
+      <c r="C309" s="9" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.15">
@@ -6980,8 +7107,8 @@
       <c r="B333" t="s">
         <v>31</v>
       </c>
-      <c r="C333" t="s">
-        <v>19</v>
+      <c r="C333" s="9" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.15">
@@ -7079,8 +7206,8 @@
       <c r="B343" t="s">
         <v>31</v>
       </c>
-      <c r="C343" t="s">
-        <v>19</v>
+      <c r="C343" s="9" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.15">
@@ -7244,8 +7371,8 @@
       <c r="B359" t="s">
         <v>31</v>
       </c>
-      <c r="C359" t="s">
-        <v>19</v>
+      <c r="C359" s="9" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.15">
@@ -7420,8 +7547,8 @@
       <c r="B376" t="s">
         <v>31</v>
       </c>
-      <c r="C376" t="s">
-        <v>19</v>
+      <c r="C376" s="9" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.15">
@@ -7585,8 +7712,8 @@
       <c r="B392" t="s">
         <v>31</v>
       </c>
-      <c r="C392" t="s">
-        <v>19</v>
+      <c r="C392" s="9" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.15">
@@ -7860,8 +7987,8 @@
       <c r="B418" t="s">
         <v>31</v>
       </c>
-      <c r="C418" t="s">
-        <v>19</v>
+      <c r="C418" s="9" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.15">
@@ -7993,8 +8120,8 @@
       <c r="B431" t="s">
         <v>31</v>
       </c>
-      <c r="C431" t="s">
-        <v>19</v>
+      <c r="C431" s="9" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.15">
@@ -8290,8 +8417,8 @@
       <c r="B459" t="s">
         <v>31</v>
       </c>
-      <c r="C459" t="s">
-        <v>19</v>
+      <c r="C459" s="9" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.15">
@@ -8466,8 +8593,8 @@
       <c r="B476" t="s">
         <v>31</v>
       </c>
-      <c r="C476" t="s">
-        <v>19</v>
+      <c r="C476" s="9" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.15">
@@ -8491,8 +8618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06ADD67-459A-3448-A388-0C190A7D0288}">
   <dimension ref="A1:D315"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A38" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8704,7 +8831,7 @@
         <v>112</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -9000,8 +9127,8 @@
       <c r="B46" t="s">
         <v>31</v>
       </c>
-      <c r="C46" t="s">
-        <v>19</v>
+      <c r="C46" s="9" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
@@ -9179,8 +9306,8 @@
       <c r="B63" t="s">
         <v>31</v>
       </c>
-      <c r="C63" t="s">
-        <v>19</v>
+      <c r="C63" s="9" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
@@ -9394,8 +9521,8 @@
       <c r="B84" t="s">
         <v>31</v>
       </c>
-      <c r="C84" t="s">
-        <v>19</v>
+      <c r="C84" s="9" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
@@ -9669,8 +9796,8 @@
       <c r="B110" t="s">
         <v>31</v>
       </c>
-      <c r="C110" t="s">
-        <v>19</v>
+      <c r="C110" s="9" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
@@ -9856,8 +9983,8 @@
       <c r="B128" t="s">
         <v>31</v>
       </c>
-      <c r="C128" t="s">
-        <v>19</v>
+      <c r="C128" s="9" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.15">
@@ -9998,8 +10125,8 @@
       <c r="B140" t="s">
         <v>31</v>
       </c>
-      <c r="C140" t="s">
-        <v>19</v>
+      <c r="C140" s="9" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.15">
@@ -10064,8 +10191,8 @@
       <c r="B147" t="s">
         <v>31</v>
       </c>
-      <c r="C147" t="s">
-        <v>19</v>
+      <c r="C147" s="9" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
@@ -10119,8 +10246,8 @@
       <c r="B153" t="s">
         <v>31</v>
       </c>
-      <c r="C153" t="s">
-        <v>19</v>
+      <c r="C153" s="9" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
@@ -10306,8 +10433,8 @@
       <c r="B171" t="s">
         <v>31</v>
       </c>
-      <c r="C171" t="s">
-        <v>19</v>
+      <c r="C171" s="9" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
@@ -10504,8 +10631,8 @@
       <c r="B190" t="s">
         <v>31</v>
       </c>
-      <c r="C190" t="s">
-        <v>19</v>
+      <c r="C190" s="9" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
@@ -10658,8 +10785,8 @@
       <c r="B205" t="s">
         <v>31</v>
       </c>
-      <c r="C205" t="s">
-        <v>19</v>
+      <c r="C205" s="9" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.15">
@@ -10746,8 +10873,8 @@
       <c r="B214" t="s">
         <v>31</v>
       </c>
-      <c r="C214" t="s">
-        <v>19</v>
+      <c r="C214" s="9" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.15">
@@ -10944,8 +11071,8 @@
       <c r="B233" t="s">
         <v>31</v>
       </c>
-      <c r="C233" t="s">
-        <v>19</v>
+      <c r="C233" s="9" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.15">
@@ -11043,8 +11170,8 @@
       <c r="B243" t="s">
         <v>31</v>
       </c>
-      <c r="C243" t="s">
-        <v>19</v>
+      <c r="C243" s="9" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.15">
@@ -11148,8 +11275,8 @@
       <c r="B253" t="s">
         <v>31</v>
       </c>
-      <c r="C253" t="s">
-        <v>19</v>
+      <c r="C253" s="9" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.15">
@@ -11346,8 +11473,8 @@
       <c r="B272" t="s">
         <v>31</v>
       </c>
-      <c r="C272" t="s">
-        <v>19</v>
+      <c r="C272" s="9" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.15">
@@ -11500,8 +11627,8 @@
       <c r="B287" t="s">
         <v>31</v>
       </c>
-      <c r="C287" t="s">
-        <v>19</v>
+      <c r="C287" s="9" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.15">
@@ -11580,8 +11707,8 @@
       <c r="B295" t="s">
         <v>31</v>
       </c>
-      <c r="C295" t="s">
-        <v>19</v>
+      <c r="C295" s="9" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
@@ -11778,8 +11905,8 @@
       <c r="B314" t="s">
         <v>31</v>
       </c>
-      <c r="C314" t="s">
-        <v>19</v>
+      <c r="C314" s="9" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.15">
@@ -11802,7 +11929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
+    <sheetView zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -11827,7 +11954,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -11839,16 +11966,16 @@
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -11856,7 +11983,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -11869,7 +11996,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -11886,7 +12013,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C4">
         <v>120</v>
@@ -11899,7 +12026,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -11917,7 +12044,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C5">
         <v>120</v>
@@ -11930,7 +12057,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -11956,7 +12083,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11980,7 +12107,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -11992,16 +12119,16 @@
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -12009,7 +12136,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C3">
         <v>40.00000000007276</v>
@@ -12021,7 +12148,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -12038,7 +12165,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C4">
         <v>14.999999999781721</v>
@@ -12050,7 +12177,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -12068,7 +12195,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C5">
         <v>25.000000000291038</v>
@@ -12080,7 +12207,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -12098,7 +12225,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C6">
         <v>34.999999999818101</v>
@@ -12110,7 +12237,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -12128,7 +12255,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C7">
         <v>29.999999999890861</v>
@@ -12140,7 +12267,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -12158,7 +12285,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="C8">
         <v>115.00000000029104</v>
@@ -12170,7 +12297,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -12188,7 +12315,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C9">
         <v>54.999999999854481</v>
@@ -12200,7 +12327,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -12218,7 +12345,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C10">
         <v>935.00000000014552</v>
@@ -12230,7 +12357,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -12248,7 +12375,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -12260,7 +12387,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -12279,86 +12406,4 @@
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4289E7A-CAF4-AC46-949F-DB1752B1DF3A}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1">
-        <v>0.57023999999999997</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>384</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="2">
-        <f>B1/86400</f>
-        <v>6.5999999999999995E-6</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="2">
-        <f>B1/(24*60)</f>
-        <v>3.9599999999999998E-4</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4">
-        <f>B3*10000</f>
-        <v>3.96</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1.8899999999999999E-5</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B7" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Pennink models (all 6) done. Clean up of mf6lab directory structure.
</commit_message>
<xml_diff>
--- a/Projects/Pennink-Model/cases/Series2/Series2.xlsx
+++ b/Projects/Pennink-Model/cases/Series2/Series2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Pennink-Model/cases/Series2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA2083F-BF10-C84B-A004-579BF6B95D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3ABD4DF-3FCD-0943-9DA6-9073164AAFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9820" yWindow="-24220" windowWidth="28180" windowHeight="16980" tabRatio="751" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="446">
   <si>
     <t>ON / OFF</t>
   </si>
@@ -1343,9 +1343,6 @@
   </si>
   <si>
     <t>SIMPLE | MODERATE | COMPLEX</t>
-  </si>
-  <si>
-    <t>SIMPLE</t>
   </si>
   <si>
     <t>METER</t>
@@ -3635,8 +3632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A326" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C344" sqref="C344"/>
+    <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3761,7 +3758,7 @@
         <v>108</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>380</v>
@@ -3808,7 +3805,7 @@
         <v>112</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -4094,7 +4091,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -4204,7 +4201,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -4358,7 +4355,7 @@
         <v>31</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -4391,7 +4388,7 @@
         <v>45</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -4545,7 +4542,7 @@
         <v>31</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -4732,7 +4729,7 @@
         <v>31</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
@@ -4908,7 +4905,7 @@
         <v>31</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
@@ -5084,7 +5081,7 @@
         <v>31</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
@@ -5271,7 +5268,7 @@
         <v>31</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.15">
@@ -5469,7 +5466,7 @@
         <v>31</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
@@ -5634,7 +5631,7 @@
         <v>31</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
@@ -5799,7 +5796,7 @@
         <v>31</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.15">
@@ -5920,7 +5917,7 @@
         <v>43</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.15">
@@ -5997,7 +5994,7 @@
         <v>31</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.15">
@@ -6052,7 +6049,7 @@
         <v>31</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.15">
@@ -6349,7 +6346,7 @@
         <v>31</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.15">
@@ -6613,7 +6610,7 @@
         <v>31</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.15">
@@ -6745,7 +6742,7 @@
         <v>31</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.15">
@@ -6822,7 +6819,7 @@
         <v>43</v>
       </c>
       <c r="C306" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.15">
@@ -6855,7 +6852,7 @@
         <v>31</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.15">
@@ -7108,7 +7105,7 @@
         <v>31</v>
       </c>
       <c r="C333" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.15">
@@ -7207,7 +7204,7 @@
         <v>31</v>
       </c>
       <c r="C343" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.15">
@@ -7372,7 +7369,7 @@
         <v>31</v>
       </c>
       <c r="C359" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.15">
@@ -7548,7 +7545,7 @@
         <v>31</v>
       </c>
       <c r="C376" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.15">
@@ -7713,7 +7710,7 @@
         <v>31</v>
       </c>
       <c r="C392" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.15">
@@ -7988,7 +7985,7 @@
         <v>31</v>
       </c>
       <c r="C418" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.15">
@@ -8121,7 +8118,7 @@
         <v>31</v>
       </c>
       <c r="C431" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.15">
@@ -8418,7 +8415,7 @@
         <v>31</v>
       </c>
       <c r="C459" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.15">
@@ -8594,7 +8591,7 @@
         <v>31</v>
       </c>
       <c r="C476" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.15">
@@ -8831,7 +8828,7 @@
         <v>112</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -9128,7 +9125,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
@@ -9307,7 +9304,7 @@
         <v>31</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
@@ -9522,7 +9519,7 @@
         <v>31</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
@@ -9797,7 +9794,7 @@
         <v>31</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
@@ -9984,7 +9981,7 @@
         <v>31</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.15">
@@ -10126,7 +10123,7 @@
         <v>31</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.15">
@@ -10192,7 +10189,7 @@
         <v>31</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
@@ -10247,7 +10244,7 @@
         <v>31</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
@@ -10434,7 +10431,7 @@
         <v>31</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
@@ -10632,7 +10629,7 @@
         <v>31</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
@@ -10786,7 +10783,7 @@
         <v>31</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.15">
@@ -10874,7 +10871,7 @@
         <v>31</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.15">
@@ -11072,7 +11069,7 @@
         <v>31</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.15">
@@ -11171,7 +11168,7 @@
         <v>31</v>
       </c>
       <c r="C243" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.15">
@@ -11276,7 +11273,7 @@
         <v>31</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.15">
@@ -11474,7 +11471,7 @@
         <v>31</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.15">
@@ -11628,7 +11625,7 @@
         <v>31</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.15">
@@ -11708,7 +11705,7 @@
         <v>31</v>
       </c>
       <c r="C295" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
@@ -11906,7 +11903,7 @@
         <v>31</v>
       </c>
       <c r="C314" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.15">
@@ -11946,7 +11943,7 @@
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.15">
@@ -11954,7 +11951,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -11966,16 +11963,16 @@
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>405</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -11983,7 +11980,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -11996,7 +11993,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -12013,7 +12010,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C4">
         <v>120</v>
@@ -12026,7 +12023,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -12044,7 +12041,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C5">
         <v>120</v>
@@ -12057,7 +12054,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -12099,7 +12096,7 @@
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.15">
@@ -12107,7 +12104,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -12119,16 +12116,16 @@
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>405</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -12136,7 +12133,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C3">
         <v>40.00000000007276</v>
@@ -12148,7 +12145,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -12165,7 +12162,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C4">
         <v>14.999999999781721</v>
@@ -12177,7 +12174,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -12195,7 +12192,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C5">
         <v>25.000000000291038</v>
@@ -12207,7 +12204,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -12225,7 +12222,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C6">
         <v>34.999999999818101</v>
@@ -12237,7 +12234,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -12255,7 +12252,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C7">
         <v>29.999999999890861</v>
@@ -12267,7 +12264,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -12285,7 +12282,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C8">
         <v>115.00000000029104</v>
@@ -12297,7 +12294,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -12315,7 +12312,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C9">
         <v>54.999999999854481</v>
@@ -12327,7 +12324,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -12345,7 +12342,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C10">
         <v>935.00000000014552</v>
@@ -12357,7 +12354,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -12375,7 +12372,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -12387,7 +12384,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G11">
         <v>0</v>

</xml_diff>